<commit_message>
Schedule fix and readme update
Corrected links
</commit_message>
<xml_diff>
--- a/Schedule/tentative_schedule.xlsx
+++ b/Schedule/tentative_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlovele/Library/CloudStorage/Dropbox/Mac (3)/Documents/GitHub/iu-vlsi/Schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329DF738-A6D4-F44B-A62A-770711512CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3208CCC7-17F0-404D-ABEC-A86C3A755FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43500" yWindow="2540" windowWidth="25300" windowHeight="17480" xr2:uid="{B06FCACC-7A90-6240-A88B-5F618B4AAD7E}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,7 +781,9 @@
       <c r="A8" s="3">
         <v>45321</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>45692</v>
+      </c>
       <c r="C8" s="4">
         <v>7</v>
       </c>
@@ -790,9 +792,6 @@
       </c>
       <c r="E8" s="5">
         <v>4.2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>9</v>
       </c>
       <c r="I8" s="8"/>
     </row>
@@ -800,7 +799,9 @@
       <c r="A9" s="3">
         <v>45323</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3">
+        <v>45694</v>
+      </c>
       <c r="C9" s="4">
         <v>8</v>
       </c>
@@ -809,6 +810,9 @@
       </c>
       <c r="E9" s="5">
         <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
       </c>
       <c r="I9" s="8"/>
     </row>

</xml_diff>